<commit_message>
Féléves beszámoló és ppt, irodalom jegyzék
</commit_message>
<xml_diff>
--- a/Dokumentumok/Adatbázisminta.xlsx
+++ b/Dokumentumok/Adatbázisminta.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SZAKDOLGOZAT\Dokumentumok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Udvardi Dávid\Szakdolgozat\Dokumentumok\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Csapatok.sql" sheetId="1" r:id="rId1"/>
@@ -460,160 +460,160 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -927,571 +927,571 @@
   <dimension ref="B1:M68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.25" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" customWidth="1"/>
-    <col min="11" max="11" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="36" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>1</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>1</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="H3" s="37" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="40"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="40"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="40"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="40"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="37"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="40"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="41"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="25">
+      <c r="B17" s="24">
         <v>1</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="25"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="36"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="36"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="36"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="34"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="36"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="36"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="36"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="36"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="26"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="36"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="52"/>
+      <c r="F26" s="49"/>
     </row>
     <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="37"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="56"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="28" t="s">
+      <c r="H29" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="28" t="s">
+      <c r="J29" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="K29" s="38" t="s">
+      <c r="K29" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="L29" s="36"/>
+      <c r="L29" s="34"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="29">
+      <c r="B30" s="28">
         <v>1</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="12">
         <v>700</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="12">
         <v>171</v>
       </c>
-      <c r="G30" s="13">
+      <c r="G30" s="12">
         <v>8.6</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="H30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="12">
         <v>1995</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="12">
         <v>1850</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="16">
         <v>5260</v>
       </c>
-      <c r="L30" s="36"/>
+      <c r="L30" s="34"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="36"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="34"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="29"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="36"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="34"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="29"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="36"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="34"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="36"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="34"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="36"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="34"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="36"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="34"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="29"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="36"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="34"/>
     </row>
     <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="30"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="36"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="34"/>
     </row>
     <row r="42" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="37"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="56"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="36"/>
+      <c r="E43" s="34"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="B44" s="55">
+    <row r="44" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="B44" s="52">
         <v>1</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="57" t="s">
+      <c r="D44" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="36"/>
+      <c r="E44" s="34"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="32"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="36"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="34"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="32"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="36"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="34"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="32"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="36"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="34"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="32"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="36"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="34"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="32"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="36"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="34"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="32"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="36"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="34"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="32"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="36"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="34"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="33"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="36"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="34"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -1504,274 +1504,274 @@
     </row>
     <row r="57" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
+      <c r="B58" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G58" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="H58" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I58" s="7" t="s">
+      <c r="I58" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J58" s="7" t="s">
+      <c r="J58" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K58" s="7" t="s">
+      <c r="K58" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L58" s="7" t="s">
+      <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M58" s="11" t="s">
+      <c r="M58" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="45">
+      <c r="B59" s="42">
         <v>1</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E59" s="13" t="s">
+      <c r="E59" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F59" s="13">
+      <c r="F59" s="12">
         <v>34</v>
       </c>
-      <c r="G59" s="13"/>
-      <c r="H59" s="42">
+      <c r="G59" s="12"/>
+      <c r="H59" s="39">
         <v>42671</v>
       </c>
-      <c r="I59" s="43">
+      <c r="I59" s="40">
         <v>42644</v>
       </c>
-      <c r="J59" s="13" t="s">
+      <c r="J59" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="17"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="16"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="45">
+      <c r="B60" s="42">
         <v>2</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D60" s="13" t="s">
+      <c r="D60" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E60" s="13" t="s">
+      <c r="E60" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F60" s="13">
+      <c r="F60" s="12">
         <v>147</v>
       </c>
-      <c r="G60" s="13"/>
-      <c r="H60" s="42">
+      <c r="G60" s="12"/>
+      <c r="H60" s="39">
         <v>42677</v>
       </c>
-      <c r="I60" s="43">
+      <c r="I60" s="40">
         <v>42649</v>
       </c>
-      <c r="J60" s="13" t="s">
+      <c r="J60" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K60" s="13"/>
-      <c r="L60" s="13"/>
-      <c r="M60" s="17"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="16"/>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B61" s="45">
+      <c r="B61" s="42">
         <v>3</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E61" s="13" t="s">
+      <c r="E61" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="13">
+      <c r="F61" s="12">
         <v>38</v>
       </c>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13" t="s">
+      <c r="G61" s="12"/>
+      <c r="H61" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="I61" s="13" t="s">
+      <c r="I61" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="J61" s="13" t="s">
+      <c r="J61" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K61" s="13"/>
-      <c r="L61" s="13"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
       <c r="M61" s="1"/>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="45">
+      <c r="B62" s="42">
         <v>4</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E62" s="13" t="s">
+      <c r="E62" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="12">
         <v>34</v>
       </c>
-      <c r="G62" s="13"/>
-      <c r="H62" s="42">
+      <c r="G62" s="12"/>
+      <c r="H62" s="39">
         <v>42663</v>
       </c>
-      <c r="I62" s="42">
+      <c r="I62" s="39">
         <v>42662</v>
       </c>
-      <c r="J62" s="13" t="s">
+      <c r="J62" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
       <c r="M62" s="1"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="45">
+      <c r="B63" s="42">
         <v>5</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E63" s="13" t="s">
+      <c r="E63" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="12">
         <v>147</v>
       </c>
-      <c r="G63" s="13"/>
-      <c r="H63" s="42">
+      <c r="G63" s="12"/>
+      <c r="H63" s="39">
         <v>42663</v>
       </c>
-      <c r="I63" s="42">
+      <c r="I63" s="39">
         <v>42662</v>
       </c>
-      <c r="J63" s="13" t="s">
+      <c r="J63" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
       <c r="M63" s="1"/>
     </row>
     <row r="64" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="46">
+      <c r="B64" s="43">
         <v>6</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="19">
+      <c r="F64" s="18">
         <v>38</v>
       </c>
-      <c r="G64" s="19"/>
-      <c r="H64" s="47">
+      <c r="G64" s="18"/>
+      <c r="H64" s="44">
         <v>42663</v>
       </c>
-      <c r="I64" s="47">
+      <c r="I64" s="44">
         <v>42662</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="J64" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
       <c r="M64" s="2"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="34"/>
-      <c r="K65" s="34"/>
-      <c r="L65" s="34"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="33"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="34"/>
-      <c r="G66" s="34"/>
-      <c r="H66" s="34"/>
-      <c r="I66" s="34"/>
-      <c r="J66" s="34"/>
-      <c r="K66" s="34"/>
-      <c r="L66" s="34"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="33"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="34"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="34"/>
-      <c r="K67" s="34"/>
-      <c r="L67" s="34"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="34"/>
-      <c r="G68" s="34"/>
-      <c r="H68" s="34"/>
-      <c r="I68" s="34"/>
-      <c r="J68" s="34"/>
-      <c r="K68" s="34"/>
-      <c r="L68" s="34"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>